<commit_message>
Previous tenure validation and better simple data csv
</commit_message>
<xml_diff>
--- a/modules/prototype-kit/codebase/testfiles/Simple Test Data.xlsx
+++ b/modules/prototype-kit/codebase/testfiles/Simple Test Data.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">5) Contract Start Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">14) Immediately prior to this letting, was this household…?:</t>
+    <t xml:space="preserve">14) Immediately prior to this letting, was this household homeless…?:</t>
   </si>
   <si>
     <t xml:space="preserve">9) What was the housing situation for this household immediately before this letting?:</t>
@@ -2557,11 +2557,11 @@
   </sheetPr>
   <dimension ref="A1:F468"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="139.44"/>

</xml_diff>